<commit_message>
Added some firmware tweals , servo motor needs a special firmware edit as well
</commit_message>
<xml_diff>
--- a/Current BOM .xlsx
+++ b/Current BOM .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AAA HACK CLUB PRJ\9. CNC 2D Plotter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AAA HACK CLUB PRJ\9. CNC 2D Plotter\Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D67288F-AC63-416A-8174-B3EB77D8CC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F94489-1941-4672-A8AA-787CCEE54AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC711047-CCCA-45F5-BAE5-73640EF9927A}"/>
   </bookViews>
@@ -226,7 +226,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -235,8 +235,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -557,13 +555,13 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
@@ -574,7 +572,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -594,7 +592,7 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" s="6">
@@ -615,14 +613,14 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>2</v>
       </c>
       <c r="C3" s="4">
         <v>5.81</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D16" si="0">SUM(B3*C3)</f>
+        <f t="shared" ref="D3:D15" si="0">SUM(B3*C3)</f>
         <v>11.62</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -636,7 +634,7 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="4"/>
@@ -664,7 +662,7 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" s="6">
@@ -682,7 +680,7 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="6">
@@ -712,7 +710,7 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="6">
@@ -730,7 +728,7 @@
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" s="6">
@@ -748,7 +746,7 @@
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" s="6">
@@ -769,7 +767,7 @@
       <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" s="6">
@@ -790,7 +788,7 @@
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="6">
@@ -808,7 +806,7 @@
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="6">
@@ -826,7 +824,7 @@
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="6">

</xml_diff>